<commit_message>
Updated Gyro and I2C
</commit_message>
<xml_diff>
--- a/Documents/PinOut.xlsx
+++ b/Documents/PinOut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Ports</t>
   </si>
@@ -102,6 +102,18 @@
   </si>
   <si>
     <t>yellow</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>Not used</t>
   </si>
 </sst>
 </file>
@@ -419,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,6 +616,40 @@
         <v>24</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented timer running a testpoint
</commit_message>
<xml_diff>
--- a/Documents/PinOut.xlsx
+++ b/Documents/PinOut.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
   <si>
     <t>Ports</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>Pin Config</t>
+  </si>
+  <si>
+    <t>TESTPOINT_0</t>
   </si>
 </sst>
 </file>
@@ -500,25 +503,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,7 +805,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,101 +890,101 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="24">
         <v>2</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="24">
         <v>47</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="26">
         <v>3</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="26">
         <v>48</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+    <row r="6" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="27">
         <v>6</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="27">
         <v>14</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G6" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+    <row r="7" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="25">
         <v>7</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="25">
         <v>13</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="25" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1016,7 +1019,7 @@
         <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1167,7 +1170,7 @@
       <c r="H2" s="1">
         <v>7</v>
       </c>
-      <c r="I2" s="23"/>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1176,15 +1179,15 @@
       <c r="B3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="23"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="31"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -1197,7 +1200,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="27"/>
+      <c r="I7" s="30"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
@@ -1210,7 +1213,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="27"/>
+      <c r="I8" s="30"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
@@ -1221,7 +1224,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
-      <c r="I9" s="27"/>
+      <c r="I9" s="30"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -1234,7 +1237,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="27"/>
+      <c r="I10" s="30"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -1247,7 +1250,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="27"/>
+      <c r="I11" s="30"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
@@ -1258,7 +1261,7 @@
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
-      <c r="I12" s="27"/>
+      <c r="I12" s="30"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
@@ -1271,7 +1274,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="27"/>
+      <c r="I13" s="30"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -1284,7 +1287,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="27"/>
+      <c r="I14" s="30"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1295,7 +1298,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="27"/>
+      <c r="I15" s="30"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
@@ -1308,7 +1311,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="27"/>
+      <c r="I16" s="30"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -1321,7 +1324,7 @@
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="27"/>
+      <c r="I17" s="30"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1332,7 +1335,7 @@
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
-      <c r="I18" s="27"/>
+      <c r="I18" s="30"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
@@ -1345,7 +1348,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="27"/>
+      <c r="I19" s="30"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
@@ -1358,7 +1361,7 @@
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
-      <c r="I20" s="27"/>
+      <c r="I20" s="30"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1369,7 +1372,7 @@
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="27"/>
+      <c r="I21" s="30"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
@@ -1382,7 +1385,7 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
-      <c r="I22" s="27"/>
+      <c r="I22" s="30"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
@@ -1395,7 +1398,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
-      <c r="I23" s="27"/>
+      <c r="I23" s="30"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
@@ -1406,7 +1409,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
-      <c r="I24" s="27"/>
+      <c r="I24" s="30"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
@@ -1418,8 +1421,8 @@
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="27" t="s">
+      <c r="H25" s="21"/>
+      <c r="I25" s="30" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1445,23 +1448,23 @@
       <c r="G26" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="25" t="s">
+      <c r="H26" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="I26" s="27"/>
+      <c r="I26" s="30"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
       <c r="B27" s="19"/>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="22"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="27"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Implementing Timers has not been verified.
!!!PWM module has been implemented!!!!
All motors are successfully outputting a servo signal
</commit_message>
<xml_diff>
--- a/Documents/PinOut.xlsx
+++ b/Documents/PinOut.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="69">
   <si>
     <t>Ports</t>
   </si>
@@ -220,6 +220,21 @@
   </si>
   <si>
     <t>TESTPOINT_0</t>
+  </si>
+  <si>
+    <t>PWM2</t>
+  </si>
+  <si>
+    <t>PWM3</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWM0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWM1 </t>
   </si>
 </sst>
 </file>
@@ -802,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,6 +1126,92 @@
       </c>
       <c r="H14" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Command 0x0500 increases one of the timers by 10us when sent Updated the Tiva Hardware. We now have bluetooth comm confirmed. 6 byte reads confirmed. ADXL init sequence is being verified but we still need to validate that we are setting everything up correctly / Interupt enable Timers are also running :)
</commit_message>
<xml_diff>
--- a/Documents/PinOut.xlsx
+++ b/Documents/PinOut.xlsx
@@ -13,7 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="TIVA Pin OUT" sheetId="1" r:id="rId1"/>
-    <sheet name="Commands" sheetId="2" r:id="rId2"/>
+    <sheet name="ADXL345 Pin Out" sheetId="3" r:id="rId2"/>
+    <sheet name="ADXL345 Reg Spec" sheetId="4" r:id="rId3"/>
+    <sheet name="Commands" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TIVA Pin OUT'!$A$1:$I$14</definedName>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
   <si>
     <t>Ports</t>
   </si>
@@ -235,6 +237,75 @@
   </si>
   <si>
     <t xml:space="preserve">PWM1 </t>
+  </si>
+  <si>
+    <t>I2C use</t>
+  </si>
+  <si>
+    <t>Name on board</t>
+  </si>
+  <si>
+    <t>QuadCopter Pin</t>
+  </si>
+  <si>
+    <t>VDD</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>vdd</t>
+  </si>
+  <si>
+    <t>gnd</t>
+  </si>
+  <si>
+    <t>rfu</t>
+  </si>
+  <si>
+    <t>vs</t>
+  </si>
+  <si>
+    <t>cs</t>
+  </si>
+  <si>
+    <t>cs!</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>means the address is 0x53 (If we tie it to VDD we would use a different address)</t>
+  </si>
+  <si>
+    <t>INT1</t>
+  </si>
+  <si>
+    <t>INT2</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>Alt Address</t>
+  </si>
+  <si>
+    <t>sdo</t>
+  </si>
+  <si>
+    <t>sda</t>
+  </si>
+  <si>
+    <t>scl/sclk</t>
+  </si>
+  <si>
+    <t>scl</t>
+  </si>
+  <si>
+    <t>This selects I2C as the comm (GND means it is set for SPI)</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -820,7 +891,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,6 +1293,210 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" t="str">
+        <f>'TIVA Pin OUT'!E5</f>
+        <v>I2C Data</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" t="str">
+        <f>'TIVA Pin OUT'!E4</f>
+        <v>I2C CLK</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">

</xml_diff>

<commit_message>
Interrupt Pin Set up for ADXL345
</commit_message>
<xml_diff>
--- a/Documents/PinOut.xlsx
+++ b/Documents/PinOut.xlsx
@@ -18,7 +18,7 @@
     <sheet name="Commands" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TIVA Pin OUT'!$A$1:$I$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TIVA Pin OUT'!$A$1:$I$15</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="94">
   <si>
     <t>Ports</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Output</t>
   </si>
   <si>
-    <t>Input Interrupt</t>
-  </si>
-  <si>
     <t>AF</t>
   </si>
   <si>
@@ -306,6 +303,15 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>ADXL345 INT 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Int 1 </t>
+  </si>
+  <si>
+    <t>Input Interrupt D6</t>
   </si>
 </sst>
 </file>
@@ -567,7 +573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -608,6 +614,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -888,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,385 +919,436 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="F1" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="33" t="s">
         <v>60</v>
-      </c>
-      <c r="H1" t="s">
-        <v>61</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="33">
+        <v>0</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33">
+        <v>17</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
+      <c r="H2" s="33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="33">
+        <v>1</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33">
+        <v>18</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="34">
+        <v>2</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="34">
+        <v>47</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="35">
+        <v>3</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="35">
+        <v>48</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="32">
+        <v>6</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="32">
+        <v>14</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="36">
+        <v>7</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="36">
+        <v>13</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="32">
+        <v>5</v>
+      </c>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="33">
+        <v>3</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="33">
+        <v>6</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="33">
+        <v>1</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="33">
+        <v>2</v>
+      </c>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="33">
+        <v>3</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="33">
+        <v>4</v>
+      </c>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="33">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="C15" s="33"/>
+      <c r="D15" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="24">
-        <v>2</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="24">
-        <v>47</v>
-      </c>
-      <c r="E4" s="24" t="s">
+      <c r="B16" s="33">
+        <v>4</v>
+      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33">
+        <v>58</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="33">
         <v>5</v>
       </c>
-      <c r="F4" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="C17" s="33"/>
+      <c r="D17" s="33">
+        <v>57</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="26">
-        <v>3</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="26">
-        <v>48</v>
-      </c>
-      <c r="E5" s="26" t="s">
+      <c r="B18" s="33">
         <v>6</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="27">
-        <v>6</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="27">
-        <v>14</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="25">
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="33">
         <v>7</v>
       </c>
-      <c r="C7" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="25">
-        <v>13</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="D15">
-        <v>58</v>
-      </c>
-      <c r="E15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>57</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="G19" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="F16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" t="s">
-        <v>54</v>
-      </c>
-      <c r="H16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" t="s">
-        <v>54</v>
-      </c>
-      <c r="H18" t="s">
-        <v>66</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I14"/>
+  <autoFilter ref="A1:I15"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1296,7 +1358,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,16 +1378,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>70</v>
       </c>
-      <c r="D1" t="s">
-        <v>71</v>
-      </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1333,7 +1395,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1341,7 +1403,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1349,7 +1411,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1357,7 +1419,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1365,7 +1427,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1373,7 +1435,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1381,16 +1443,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
         <v>78</v>
       </c>
-      <c r="C8" t="s">
-        <v>79</v>
-      </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1398,7 +1460,14 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" t="str">
+        <f>'TIVA Pin OUT'!E10</f>
+        <v>Input Interrupt D6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1406,7 +1475,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1414,7 +1483,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1422,7 +1491,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1430,16 +1499,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
         <v>85</v>
       </c>
-      <c r="C13" t="s">
-        <v>86</v>
-      </c>
       <c r="D13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" t="s">
         <v>80</v>
-      </c>
-      <c r="E13" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1447,10 +1516,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" t="str">
         <f>'TIVA Pin OUT'!E5</f>
@@ -1462,10 +1531,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" t="s">
         <v>88</v>
-      </c>
-      <c r="C15" t="s">
-        <v>89</v>
       </c>
       <c r="D15" t="str">
         <f>'TIVA Pin OUT'!E4</f>
@@ -1487,7 +1556,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1512,13 +1581,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1550,13 +1619,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="28" t="s">
         <v>47</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>48</v>
       </c>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
@@ -1567,7 +1636,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1580,7 +1649,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="6"/>
@@ -1604,7 +1673,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1617,7 +1686,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="6"/>
@@ -1641,7 +1710,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -1654,7 +1723,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="6"/>
@@ -1678,7 +1747,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -1691,7 +1760,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="6"/>
@@ -1715,7 +1784,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1728,7 +1797,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="6"/>
@@ -1752,7 +1821,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1765,7 +1834,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="6"/>
@@ -1789,7 +1858,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -1799,33 +1868,33 @@
       <c r="G25" s="16"/>
       <c r="H25" s="21"/>
       <c r="I25" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>54</v>
-      </c>
       <c r="F26" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H26" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I26" s="30"/>
     </row>
@@ -1833,7 +1902,7 @@
       <c r="A27" s="18"/>
       <c r="B27" s="19"/>
       <c r="C27" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D27" s="29"/>
       <c r="E27" s="20"/>

</xml_diff>

<commit_message>
Changed clock to be sourced from PLL at 50MHz. PLL is at 200MHz
</commit_message>
<xml_diff>
--- a/Documents/PinOut.xlsx
+++ b/Documents/PinOut.xlsx
@@ -18,7 +18,7 @@
     <sheet name="Commands" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TIVA Pin OUT'!$A$1:$I$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TIVA Pin OUT'!$A$1:$I$18</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="97">
   <si>
     <t>Ports</t>
   </si>
@@ -305,20 +305,29 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>ADXL345 INT 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Int 1 </t>
   </si>
   <si>
     <t>Input Interrupt D6</t>
+  </si>
+  <si>
+    <t>NOT ACCESSIBLE ON TIVA BOARD</t>
+  </si>
+  <si>
+    <t>May be another pin for one of the motors…</t>
+  </si>
+  <si>
+    <t>TESTPOINT_1</t>
+  </si>
+  <si>
+    <t>ADXL345 INT 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,8 +335,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,6 +412,21 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -570,10 +615,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -602,6 +650,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -614,13 +670,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -899,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,34 +969,33 @@
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="29" t="s">
         <v>60</v>
       </c>
       <c r="I1" t="s">
@@ -948,407 +1003,477 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="29">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33">
+      <c r="C2" s="29"/>
+      <c r="D2" s="29">
         <v>17</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33" t="s">
+      <c r="F2" s="29"/>
+      <c r="G2" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="29" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="29">
         <v>1</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29">
         <v>18</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="29" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="29">
+        <v>2</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="34">
+      <c r="B5" s="30">
         <v>2</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C5" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D5" s="30">
         <v>47</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G5" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H5" s="30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+    <row r="6" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="35">
+      <c r="B6" s="31">
         <v>3</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C6" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D6" s="31">
         <v>48</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F6" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G6" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="35" t="s">
+      <c r="H6" s="31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+    <row r="7" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="29">
+        <v>4</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29">
+        <v>58</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7"/>
+    </row>
+    <row r="8" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="29">
+        <v>5</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29">
+        <v>57</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="29">
+        <v>6</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="29">
+        <v>7</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B11" s="28">
         <v>6</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C11" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D11" s="28">
         <v>14</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E11" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="33" t="s">
+      <c r="F11" s="28"/>
+      <c r="G11" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="32" t="s">
+      <c r="H11" s="28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+      <c r="I11" s="27"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B12" s="32">
         <v>7</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C12" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D12" s="32">
         <v>13</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E12" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36" t="s">
+      <c r="F12" s="32"/>
+      <c r="G12" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="H12" s="32" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="32">
-        <v>5</v>
-      </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32" t="s">
+      <c r="B13" s="29">
+        <v>0</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="29">
+        <v>3</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="32" t="s">
+      <c r="F14" s="29"/>
+      <c r="G14" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="34" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="33">
-        <v>3</v>
-      </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="33">
-        <v>6</v>
-      </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="33" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="33">
-        <v>1</v>
-      </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="33">
-        <v>2</v>
-      </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="33">
-        <v>3</v>
-      </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="33">
-        <v>4</v>
-      </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="33" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B15" s="33">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C15" s="33"/>
-      <c r="D15" s="33" t="s">
-        <v>23</v>
-      </c>
+      <c r="D15" s="33"/>
       <c r="E15" s="33" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F15" s="33"/>
       <c r="G15" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" s="27"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="29">
+        <v>6</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="29">
+        <v>7</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="H17" s="29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="29">
+        <v>0</v>
+      </c>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="29">
+        <v>1</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="29">
+        <v>2</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="29">
+        <v>3</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="29">
         <v>4</v>
       </c>
-      <c r="B16" s="33">
-        <v>4</v>
-      </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33">
-        <v>58</v>
-      </c>
-      <c r="E16" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="33" t="s">
+      <c r="C22" s="29"/>
+      <c r="D22" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="33">
-        <v>5</v>
-      </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33">
-        <v>57</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="33" t="s">
+      <c r="H22" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="33">
-        <v>6</v>
-      </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="33">
-        <v>7</v>
-      </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="33" t="s">
-        <v>65</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I15"/>
+  <autoFilter ref="A1:I18">
+    <sortState ref="A2:I21">
+      <sortCondition ref="A1:A17"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1358,7 +1483,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H8" sqref="E8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1463,11 +1588,11 @@
         <v>81</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" t="str">
-        <f>'TIVA Pin OUT'!E10</f>
-        <v>Input Interrupt D6</v>
+        <f>'TIVA Pin OUT'!E12</f>
+        <v>UART3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1521,8 +1646,8 @@
       <c r="C14" t="s">
         <v>86</v>
       </c>
-      <c r="D14" t="str">
-        <f>'TIVA Pin OUT'!E5</f>
+      <c r="D14" s="40" t="str">
+        <f>'TIVA Pin OUT'!E6</f>
         <v>I2C Data</v>
       </c>
     </row>
@@ -1536,8 +1661,8 @@
       <c r="C15" t="s">
         <v>88</v>
       </c>
-      <c r="D15" t="str">
-        <f>'TIVA Pin OUT'!E4</f>
+      <c r="D15" s="41" t="str">
+        <f>'TIVA Pin OUT'!E5</f>
         <v>I2C CLK</v>
       </c>
     </row>
@@ -1615,7 +1740,7 @@
       <c r="H2" s="1">
         <v>7</v>
       </c>
-      <c r="I2" s="31"/>
+      <c r="I2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1624,15 +1749,15 @@
       <c r="B3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="31"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="39"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -1645,7 +1770,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="30"/>
+      <c r="I7" s="38"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
@@ -1658,7 +1783,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="30"/>
+      <c r="I8" s="38"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
@@ -1669,7 +1794,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
-      <c r="I9" s="30"/>
+      <c r="I9" s="38"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -1682,7 +1807,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="30"/>
+      <c r="I10" s="38"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -1695,7 +1820,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="30"/>
+      <c r="I11" s="38"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
@@ -1706,7 +1831,7 @@
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
-      <c r="I12" s="30"/>
+      <c r="I12" s="38"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
@@ -1719,7 +1844,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="30"/>
+      <c r="I13" s="38"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -1732,7 +1857,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="30"/>
+      <c r="I14" s="38"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1743,7 +1868,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="30"/>
+      <c r="I15" s="38"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
@@ -1756,7 +1881,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="30"/>
+      <c r="I16" s="38"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -1769,7 +1894,7 @@
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="30"/>
+      <c r="I17" s="38"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1780,7 +1905,7 @@
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
-      <c r="I18" s="30"/>
+      <c r="I18" s="38"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
@@ -1793,7 +1918,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="30"/>
+      <c r="I19" s="38"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
@@ -1806,7 +1931,7 @@
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
-      <c r="I20" s="30"/>
+      <c r="I20" s="38"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1817,7 +1942,7 @@
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="30"/>
+      <c r="I21" s="38"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
@@ -1830,7 +1955,7 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
-      <c r="I22" s="30"/>
+      <c r="I22" s="38"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
@@ -1843,7 +1968,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
-      <c r="I23" s="30"/>
+      <c r="I23" s="38"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
@@ -1854,7 +1979,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
-      <c r="I24" s="30"/>
+      <c r="I24" s="38"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
@@ -1867,7 +1992,7 @@
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
       <c r="H25" s="21"/>
-      <c r="I25" s="30" t="s">
+      <c r="I25" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1896,20 +2021,20 @@
       <c r="H26" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="I26" s="30"/>
+      <c r="I26" s="38"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
       <c r="B27" s="19"/>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="29"/>
+      <c r="D27" s="37"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="23"/>
-      <c r="I27" s="30"/>
+      <c r="I27" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Implemented scheduler which gets the servos happy.
Successfully Starting motors with a COMMAND_LEVEL and receiving data.
Next Step Filtering
</commit_message>
<xml_diff>
--- a/Documents/PinOut.xlsx
+++ b/Documents/PinOut.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TIVA Pin OUT" sheetId="1" r:id="rId1"/>
-    <sheet name="ADXL345 Pin Out" sheetId="3" r:id="rId2"/>
-    <sheet name="ADXL345 Reg Spec" sheetId="4" r:id="rId3"/>
-    <sheet name="Commands" sheetId="2" r:id="rId4"/>
+    <sheet name="HC05 Commands" sheetId="2" r:id="rId2"/>
+    <sheet name="ADXL345 Pin Out" sheetId="3" r:id="rId3"/>
+    <sheet name="ADXL345 Reg Spec" sheetId="4" r:id="rId4"/>
+    <sheet name="Part List" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TIVA Pin OUT'!$A$1:$I$18</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="110">
   <si>
     <t>Ports</t>
   </si>
@@ -321,6 +322,47 @@
   </si>
   <si>
     <t>ADXL345 INT 2</t>
+  </si>
+  <si>
+    <t>Hobbywing</t>
+  </si>
+  <si>
+    <t>FlyFun</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>ESC</t>
+  </si>
+  <si>
+    <t>Quadcopter Use</t>
+  </si>
+  <si>
+    <t>18A, 2-4 Lipo</t>
+  </si>
+  <si>
+    <t>0x00</t>
+  </si>
+  <si>
+    <t>COMMAND_LEVEL</t>
+  </si>
+  <si>
+    <t>0x0C</t>
+  </si>
+  <si>
+    <t>Sends all motors to the same level. 
+0 = Min level 
+FFFF = MAX LEVEL</t>
+  </si>
+  <si>
+    <t>%power = level/FFFF</t>
   </si>
 </sst>
 </file>
@@ -357,7 +399,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,6 +469,30 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -621,7 +687,7 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -658,6 +724,8 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -670,8 +738,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -957,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,7 +1211,7 @@
       <c r="G7" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="42" t="s">
         <v>65</v>
       </c>
       <c r="I7"/>
@@ -1163,7 +1236,7 @@
       <c r="G8" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="43" t="s">
         <v>65</v>
       </c>
       <c r="I8"/>
@@ -1186,7 +1259,7 @@
       <c r="G9" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="44" t="s">
         <v>65</v>
       </c>
       <c r="I9"/>
@@ -1209,7 +1282,7 @@
       <c r="G10" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="34" t="s">
+      <c r="H10" s="45" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1475,10 +1548,434 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="108.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1">
+        <v>7</v>
+      </c>
+      <c r="I2" s="41"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="41"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="40"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="40"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="40"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="40"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="40"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="40"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="40"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="40"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="40"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="40"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="40"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="40"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="40"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="40"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="40"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="40"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="40"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="40"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="I26" s="40"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="18"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="39"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="40"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="46" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="I29" s="40"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="18"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="39"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="I22:I24"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="I10:I12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
@@ -1646,7 +2143,7 @@
       <c r="C14" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="40" t="str">
+      <c r="D14" s="36" t="str">
         <f>'TIVA Pin OUT'!E6</f>
         <v>I2C Data</v>
       </c>
@@ -1661,7 +2158,7 @@
       <c r="C15" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="41" t="str">
+      <c r="D15" s="37" t="str">
         <f>'TIVA Pin OUT'!E5</f>
         <v>I2C CLK</v>
       </c>
@@ -1671,7 +2168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1689,366 +2186,55 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="108.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1">
-        <v>7</v>
-      </c>
-      <c r="I2" s="39"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="39"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="38"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="38"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="38"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="38"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="38"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="38"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="38"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="38"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="38"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="38"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="38"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="38"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="38"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="38"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="38"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="38"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="38"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="38"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="38" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H26" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="I26" s="38"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="37"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="38"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="I19:I21"/>
-    <mergeCell ref="I22:I24"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="I10:I12"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a power command so that we can send a 16 bit value commanded level
</commit_message>
<xml_diff>
--- a/Documents/PinOut.xlsx
+++ b/Documents/PinOut.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TIVA Pin OUT" sheetId="1" r:id="rId1"/>
     <sheet name="HC05 Commands" sheetId="2" r:id="rId2"/>
     <sheet name="ADXL345 Pin Out" sheetId="3" r:id="rId3"/>
     <sheet name="ADXL345 Reg Spec" sheetId="4" r:id="rId4"/>
-    <sheet name="Part List" sheetId="5" r:id="rId5"/>
+    <sheet name="Gyro Pinout" sheetId="6" r:id="rId5"/>
+    <sheet name="Part List" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TIVA Pin OUT'!$A$1:$I$18</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="112">
   <si>
     <t>Ports</t>
   </si>
@@ -132,9 +133,6 @@
     <t>UART3</t>
   </si>
   <si>
-    <t xml:space="preserve">COMMAND_UP      </t>
-  </si>
-  <si>
     <t>0x05</t>
   </si>
   <si>
@@ -150,21 +148,6 @@
     <t>0x09</t>
   </si>
   <si>
-    <t>COMMAND_ON</t>
-  </si>
-  <si>
-    <t>COMMAND_OFF</t>
-  </si>
-  <si>
-    <t>COMMAND_RIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMMAND_LEFT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMMAND_DOWN    </t>
-  </si>
-  <si>
     <t>Data Packet Structure</t>
   </si>
   <si>
@@ -180,9 +163,6 @@
     <t>8 Byte Max</t>
   </si>
   <si>
-    <t>COMMAND_DELAY</t>
-  </si>
-  <si>
     <t>0x0B</t>
   </si>
   <si>
@@ -349,9 +329,6 @@
   </si>
   <si>
     <t>0x00</t>
-  </si>
-  <si>
-    <t>COMMAND_LEVEL</t>
   </si>
   <si>
     <t>0x0C</t>
@@ -363,6 +340,36 @@
   </si>
   <si>
     <t>%power = level/FFFF</t>
+  </si>
+  <si>
+    <t>SubCommand</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>COMMAND</t>
+  </si>
+  <si>
+    <t>LEVEL</t>
+  </si>
+  <si>
+    <t>DELAY</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>RIGHT</t>
+  </si>
+  <si>
+    <t>LEFT</t>
+  </si>
+  <si>
+    <t>DOWN</t>
   </si>
 </sst>
 </file>
@@ -687,7 +694,7 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -723,28 +730,26 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1031,7 +1036,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,158 +1068,166 @@
         <v>2</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="29">
-        <v>0</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29">
-        <v>17</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>21</v>
-      </c>
+      <c r="A2" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="32">
+        <v>7</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="32">
+        <v>13</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="29">
-        <v>1</v>
-      </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29">
-        <v>18</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="29"/>
+      <c r="A3" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="28">
+        <v>6</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="28">
+        <v>14</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="28"/>
       <c r="G3" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="29" t="s">
-        <v>21</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
+      <c r="D4" s="29">
+        <v>17</v>
+      </c>
       <c r="E4" s="29" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F4" s="29"/>
       <c r="G4" s="29" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>95</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="29">
+        <v>1</v>
+      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29">
+        <v>18</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5"/>
+    </row>
+    <row r="6" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B6" s="30">
         <v>2</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C6" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D6" s="30">
         <v>47</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E6" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F6" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="30" t="s">
+      <c r="G6" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="30" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="I6" s="24"/>
+    </row>
+    <row r="7" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B7" s="31">
         <v>3</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C7" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D7" s="31">
         <v>48</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F7" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="31" t="s">
+      <c r="G7" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="31" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="29">
-        <v>4</v>
-      </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29">
-        <v>58</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7"/>
+      <c r="I7" s="26"/>
     </row>
     <row r="8" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
@@ -1228,16 +1241,16 @@
         <v>57</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="43" t="s">
-        <v>65</v>
+        <v>46</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>58</v>
       </c>
       <c r="I8"/>
     </row>
@@ -1246,225 +1259,221 @@
         <v>4</v>
       </c>
       <c r="B9" s="29">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
+      <c r="D9" s="29">
+        <v>58</v>
+      </c>
       <c r="E9" s="29" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="44" t="s">
-        <v>65</v>
+        <v>46</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>58</v>
       </c>
       <c r="I9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="29">
+        <v>0</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="29">
         <v>4</v>
       </c>
-      <c r="B10" s="29">
-        <v>7</v>
-      </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="45" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="28">
-        <v>6</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="28">
-        <v>14</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="28"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="29"/>
       <c r="G11" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="27"/>
+        <v>46</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="32">
-        <v>7</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="32">
-        <v>13</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="25"/>
+      <c r="A12" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="29">
+        <v>2</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B13" s="29">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="29"/>
       <c r="E13" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="29"/>
+        <v>59</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>12</v>
+      </c>
       <c r="G13" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="35" t="s">
-        <v>94</v>
+        <v>46</v>
+      </c>
+      <c r="H13" s="44" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="29">
         <v>7</v>
-      </c>
-      <c r="B14" s="29">
-        <v>3</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
       <c r="E14" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="29"/>
+        <v>60</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>12</v>
+      </c>
       <c r="G14" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="34" t="s">
-        <v>62</v>
+        <v>46</v>
+      </c>
+      <c r="H14" s="37" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="33">
-        <v>5</v>
-      </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="H15" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="I15" s="27"/>
+      <c r="B15" s="29">
+        <v>0</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="43" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="29">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C16" s="29"/>
       <c r="D16" s="29"/>
       <c r="E16" s="29" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
       <c r="F16" s="29"/>
       <c r="G16" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="33">
+        <v>5</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="27"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
-        <v>13</v>
-      </c>
       <c r="B18" s="29">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C18" s="29"/>
-      <c r="D18" s="29" t="s">
-        <v>23</v>
-      </c>
+      <c r="D18" s="29"/>
       <c r="E18" s="29" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B19" s="29">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="29"/>
@@ -1473,18 +1482,18 @@
       </c>
       <c r="F19" s="29"/>
       <c r="G19" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="34" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="H19" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="29"/>
@@ -1493,18 +1502,18 @@
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="29" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H20" s="34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -1513,38 +1522,36 @@
       </c>
       <c r="F21" s="29"/>
       <c r="G21" s="29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>13</v>
       </c>
       <c r="B22" s="29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" s="29"/>
-      <c r="D22" s="29" t="s">
-        <v>23</v>
-      </c>
+      <c r="D22" s="29"/>
       <c r="E22" s="29" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="H22" s="29" t="s">
-        <v>53</v>
+        <v>15</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I18">
-    <sortState ref="A2:I21">
-      <sortCondition ref="A1:A17"/>
+    <sortState ref="A2:I22">
+      <sortCondition ref="D1:D18"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1554,422 +1561,485 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="108.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>3</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>4</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>5</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>6</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>7</v>
       </c>
-      <c r="I2" s="41"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="42"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
       <c r="I3" s="41"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="42"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="7"/>
+        <v>104</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>103</v>
+      </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="40"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" s="7"/>
+      <c r="J7" s="39"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="6"/>
+        <v>98</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="40"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" s="6"/>
+      <c r="J8" s="39"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
-      <c r="I9" s="40"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" s="11"/>
+      <c r="J9" s="39"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="7"/>
+        <v>104</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>111</v>
+      </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="40"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="7"/>
+      <c r="J10" s="39"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="6"/>
+        <v>98</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="4"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="40"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" s="6"/>
+      <c r="J11" s="39"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
-      <c r="I12" s="40"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12" s="11"/>
+      <c r="J12" s="39"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="7"/>
+        <v>104</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>110</v>
+      </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="40"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="7"/>
+      <c r="J13" s="39"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="6"/>
+        <v>98</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="4"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="40"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="6"/>
+      <c r="J14" s="39"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="40"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="11"/>
+      <c r="J15" s="39"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="7"/>
+        <v>104</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>109</v>
+      </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="40"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="7"/>
+      <c r="J16" s="39"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="6"/>
+        <v>98</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="4"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="40"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="6"/>
+      <c r="J17" s="39"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
-      <c r="I18" s="40"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="11"/>
+      <c r="J18" s="39"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="7"/>
+        <v>104</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="40"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="7"/>
+      <c r="J19" s="39"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C20" s="6"/>
+        <v>98</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
-      <c r="I20" s="40"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="6"/>
+      <c r="J20" s="39"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="40"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="5"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="39"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>107</v>
+      </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
-      <c r="I22" s="40"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="5"/>
+      <c r="J22" s="39"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="6"/>
+        <v>98</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="4"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
-      <c r="I23" s="40"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I23" s="6"/>
+      <c r="J23" s="39"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="4"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
-      <c r="I24" s="40"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="16"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="39"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>106</v>
+      </c>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="40" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>54</v>
+      <c r="H25" s="16"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H26" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="I26" s="40"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I26" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" s="39"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="39"/>
-      <c r="E27" s="20"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="40"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="40"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="B28" s="16"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="39"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>105</v>
+      </c>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="46" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>54</v>
+      <c r="H28" s="16"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H29" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="I29" s="40"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J29" s="39"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" s="39"/>
-      <c r="E30" s="20"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" s="40"/>
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="40"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="I19:I21"/>
-    <mergeCell ref="I22:I24"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="J19:J21"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="J10:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1980,7 +2050,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="E8:H8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2000,16 +2070,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2017,7 +2087,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2025,7 +2095,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2033,7 +2103,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2041,7 +2111,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2049,7 +2119,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2057,7 +2127,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2065,16 +2135,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2082,14 +2152,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" t="str">
-        <f>'TIVA Pin OUT'!E12</f>
-        <v>UART3</v>
+        <v>84</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2097,7 +2166,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2105,7 +2174,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2113,7 +2182,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2121,16 +2190,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2138,14 +2207,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="36" t="str">
-        <f>'TIVA Pin OUT'!E6</f>
-        <v>I2C Data</v>
+        <v>79</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2153,14 +2221,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="37" t="str">
-        <f>'TIVA Pin OUT'!E5</f>
-        <v>I2C CLK</v>
+        <v>81</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2178,7 +2245,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2187,6 +2254,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2205,33 +2284,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" t="s">
         <v>97</v>
-      </c>
-      <c r="C4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Interrupt and init set up for gyro. Currently sampling accel and gyro at 100hz asynchronously. next steps are synchronous sampling and a filter
</commit_message>
<xml_diff>
--- a/Documents/PinOut.xlsx
+++ b/Documents/PinOut.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TIVA Pin OUT" sheetId="1" r:id="rId1"/>
     <sheet name="HC05 Commands" sheetId="2" r:id="rId2"/>
     <sheet name="ADXL345 Pin Out" sheetId="3" r:id="rId3"/>
     <sheet name="ADXL345 Reg Spec" sheetId="4" r:id="rId4"/>
-    <sheet name="Gyro Pinout" sheetId="6" r:id="rId5"/>
-    <sheet name="Part List" sheetId="5" r:id="rId6"/>
+    <sheet name="Gyro L3GD20H" sheetId="7" r:id="rId5"/>
+    <sheet name="Gyro Reg Spec" sheetId="8" r:id="rId6"/>
+    <sheet name="Part List" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TIVA Pin OUT'!$A$1:$I$18</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="145">
   <si>
     <t>Ports</t>
   </si>
@@ -370,6 +371,116 @@
   </si>
   <si>
     <t>DOWN</t>
+  </si>
+  <si>
+    <t>Pin #</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Quadcopter</t>
+  </si>
+  <si>
+    <t>VDD IO</t>
+  </si>
+  <si>
+    <t>Power Supply for IO pins</t>
+  </si>
+  <si>
+    <t>SCL
+SPC</t>
+  </si>
+  <si>
+    <t>I2C serial clock (SCL)
+SPI serial port clock (SPC)</t>
+  </si>
+  <si>
+    <t>I2C Clock</t>
+  </si>
+  <si>
+    <t>I2C serial data (SDA)
+SPI serial data input (SDI)
+3-wire interface serial data output (SDO)</t>
+  </si>
+  <si>
+    <t>SDA
+SDI
+SDO</t>
+  </si>
+  <si>
+    <t>SDO
+SA0</t>
+  </si>
+  <si>
+    <t>SPI serial data output (SDO)
+I2C less significant bit of the device address (SA0)</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>I2C/SPI mode selection (1: SPI idle mode / I2C communication
+enabled; 0: SPI communication mode / I2C disabled)</t>
+  </si>
+  <si>
+    <t>DRDY/INT2</t>
+  </si>
+  <si>
+    <t>Data ready/fifo interrupt (FIFO threshold/overrun/empty)</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>Connect to GND with ceramic capacitor(3)</t>
+  </si>
+  <si>
+    <t>Programmable interrupt</t>
+  </si>
+  <si>
+    <t>Power Supply</t>
+  </si>
+  <si>
+    <t>25V 10nF</t>
+  </si>
+  <si>
+    <t>VDD (10uF cap)</t>
+  </si>
+  <si>
+    <t>Gyroscope data enable 
+(connect to ground if DEN is not used)</t>
+  </si>
+  <si>
+    <t>FIFO Bypass Mode</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Reg</t>
+  </si>
+  <si>
+    <t>I2C Mode</t>
+  </si>
+  <si>
+    <t>Tied to GND - Address = 1101010 = 0x6A 
+(if tied to VDD address would be 0x6B)</t>
+  </si>
+  <si>
+    <t>INVALID_COMMAND</t>
+  </si>
+  <si>
+    <t>0xFF</t>
   </si>
 </sst>
 </file>
@@ -406,7 +517,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -500,6 +611,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -694,7 +811,7 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -733,6 +850,8 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -748,8 +867,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1361,7 +1502,7 @@
       <c r="G13" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="44" t="s">
+      <c r="H13" s="39" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1403,7 +1544,7 @@
       <c r="G15" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="43" t="s">
+      <c r="H15" s="38" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1563,13 +1704,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="1" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="65.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1614,7 +1760,7 @@
       <c r="I2" s="1">
         <v>7</v>
       </c>
-      <c r="J2" s="42"/>
+      <c r="J2" s="44"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1626,15 +1772,29 @@
       <c r="C3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="8"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -1650,7 +1810,7 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="39"/>
+      <c r="J7" s="41"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
@@ -1659,14 +1819,16 @@
       <c r="B8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="39"/>
+      <c r="J8" s="41"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
@@ -1678,7 +1840,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="39"/>
+      <c r="J9" s="41"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -1694,7 +1856,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="39"/>
+      <c r="J10" s="41"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -1703,14 +1865,16 @@
       <c r="B11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="39"/>
+      <c r="J11" s="41"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
@@ -1722,7 +1886,7 @@
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
-      <c r="J12" s="39"/>
+      <c r="J12" s="41"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
@@ -1738,7 +1902,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="39"/>
+      <c r="J13" s="41"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -1747,14 +1911,16 @@
       <c r="B14" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="39"/>
+      <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1766,7 +1932,7 @@
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
-      <c r="J15" s="39"/>
+      <c r="J15" s="41"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
@@ -1782,7 +1948,7 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="39"/>
+      <c r="J16" s="41"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -1791,14 +1957,16 @@
       <c r="B17" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="39"/>
+      <c r="J17" s="41"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1810,7 +1978,7 @@
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
-      <c r="J18" s="39"/>
+      <c r="J18" s="41"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
@@ -1826,7 +1994,7 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="39"/>
+      <c r="J19" s="41"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
@@ -1844,7 +2012,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="39"/>
+      <c r="J20" s="41"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -1856,7 +2024,7 @@
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
-      <c r="J21" s="39"/>
+      <c r="J21" s="41"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
@@ -1872,7 +2040,7 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="39"/>
+      <c r="J22" s="41"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
@@ -1881,14 +2049,16 @@
       <c r="B23" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
-      <c r="J23" s="39"/>
+      <c r="J23" s="41"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
@@ -1900,7 +2070,7 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="39"/>
+      <c r="J24" s="41"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
@@ -1916,7 +2086,7 @@
       <c r="G25" s="16"/>
       <c r="H25" s="16"/>
       <c r="I25" s="21"/>
-      <c r="J25" s="39" t="s">
+      <c r="J25" s="41" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1948,21 +2118,21 @@
       <c r="I26" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="J26" s="39"/>
+      <c r="J26" s="41"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="19"/>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="40"/>
+      <c r="E27" s="42"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
       <c r="I27" s="23"/>
-      <c r="J27" s="39"/>
+      <c r="J27" s="41"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
@@ -1978,7 +2148,7 @@
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
       <c r="I28" s="21"/>
-      <c r="J28" s="38" t="s">
+      <c r="J28" s="40" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2010,21 +2180,21 @@
       <c r="I29" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="J29" s="39"/>
+      <c r="J29" s="41"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="E30" s="40"/>
+      <c r="E30" s="42"/>
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
       <c r="I30" s="23"/>
-      <c r="J30" s="39"/>
+      <c r="J30" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2255,17 +2425,290 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="47" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="47"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="45">
+        <v>1</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="45">
+        <v>2</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="45">
+        <v>3</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="45">
+        <v>4</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="45">
+        <v>5</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="45">
+        <v>6</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="45"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="45">
+        <v>7</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" s="45"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="45">
+        <v>8</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="45">
+        <v>9</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="45"/>
+      <c r="D10" s="49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="45">
+        <v>10</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="45"/>
+      <c r="D11" s="49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="45">
+        <v>11</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="45"/>
+      <c r="D12" s="49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="45">
+        <v>12</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="45"/>
+      <c r="D13" s="49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="45">
+        <v>13</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="45"/>
+      <c r="D14" s="49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="45">
+        <v>14</v>
+      </c>
+      <c r="B15" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="45">
+        <v>15</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="45"/>
+      <c r="D16" s="49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="45">
+        <v>16</v>
+      </c>
+      <c r="B17" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" s="50" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>

</xml_diff>